<commit_message>
updates from the laptop
</commit_message>
<xml_diff>
--- a/NFP/Simulation/201411/FinalEnsemble/FinalEnsenble.xlsx
+++ b/NFP/Simulation/201411/FinalEnsemble/FinalEnsenble.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuzhan\Git\Predictions\NFP\Simulation\201411\FinalEnsemble\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuzhan\git\Predictions\NFP\Simulation\201411\FinalEnsemble\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,31 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="FinalEnsemble" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Month</t>
   </si>
   <si>
     <t>L1</t>
-  </si>
-  <si>
-    <t>bootstrapping</t>
-  </si>
-  <si>
-    <t>cv</t>
-  </si>
-  <si>
-    <t>random sampling - 3 features</t>
-  </si>
-  <si>
-    <t>single combo - model 1,4,6</t>
   </si>
   <si>
     <t>Bootstrapping (9/14)</t>
@@ -47,15 +34,6 @@
   </si>
   <si>
     <t>Random Sampling of Best Features (9/14)</t>
-  </si>
-  <si>
-    <t>Single Combo 1 (9/14)</t>
-  </si>
-  <si>
-    <t>Single Combo 4 (8/14)</t>
-  </si>
-  <si>
-    <t>Single Combo 6 (11/14)</t>
   </si>
   <si>
     <t>Ensemble</t>
@@ -73,17 +51,32 @@
     <t>MWin</t>
   </si>
   <si>
-    <t>Single Combo 2 (9/14)</t>
+    <t>Dwin (10/14)</t>
   </si>
   <si>
-    <t>Dwin (10/14)</t>
+    <t>Ensemble of IJC Models (11/14)</t>
+  </si>
+  <si>
+    <t>AR Model (9/14)</t>
+  </si>
+  <si>
+    <t>Ensemble of Consensus Models (7/14)</t>
+  </si>
+  <si>
+    <t>Best Features (9/14)</t>
+  </si>
+  <si>
+    <t>Baseline Model</t>
+  </si>
+  <si>
+    <t>Dwin (6/14)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,14 +215,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -580,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -902,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,10 +898,10 @@
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -924,25 +909,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -959,16 +944,16 @@
         <v>207.42057784644101</v>
       </c>
       <c r="E2">
+        <v>239.01932921584699</v>
+      </c>
+      <c r="F2">
+        <v>262.916732099179</v>
+      </c>
+      <c r="G2">
         <v>257.23306705018803</v>
       </c>
-      <c r="F2">
-        <v>329.817465806087</v>
-      </c>
-      <c r="G2">
-        <v>320.00317096373402</v>
-      </c>
       <c r="H2">
-        <v>325.16113526329502</v>
+        <v>138.96437644244901</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -985,16 +970,16 @@
         <v>142.553462801308</v>
       </c>
       <c r="E3">
+        <v>188.56202590483099</v>
+      </c>
+      <c r="F3">
+        <v>137.73743218503299</v>
+      </c>
+      <c r="G3">
         <v>176.906973494997</v>
       </c>
-      <c r="F3">
-        <v>160.88496762064801</v>
-      </c>
-      <c r="G3">
-        <v>130.84152079971</v>
-      </c>
       <c r="H3">
-        <v>188.56202590483099</v>
+        <v>139.37666509518201</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1011,16 +996,16 @@
         <v>199.60767102854501</v>
       </c>
       <c r="E4">
+        <v>203.16213387210601</v>
+      </c>
+      <c r="F4">
+        <v>184.376068383101</v>
+      </c>
+      <c r="G4">
         <v>246.670140706588</v>
       </c>
-      <c r="F4">
-        <v>207.92631873246401</v>
-      </c>
-      <c r="G4">
-        <v>175.03749524187799</v>
-      </c>
       <c r="H4">
-        <v>203.16213387210601</v>
+        <v>168.24495681380199</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1037,16 +1022,16 @@
         <v>143.093997854478</v>
       </c>
       <c r="E5">
+        <v>147.11360038661499</v>
+      </c>
+      <c r="F5">
+        <v>174.45796030287701</v>
+      </c>
+      <c r="G5">
         <v>106.45511985007001</v>
       </c>
-      <c r="F5">
-        <v>183.106072198558</v>
-      </c>
-      <c r="G5">
-        <v>57.019400051926603</v>
-      </c>
       <c r="H5">
-        <v>160.60802092857301</v>
+        <v>190.19757033262101</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1063,16 +1048,16 @@
         <v>166.16294779456999</v>
       </c>
       <c r="E6">
+        <v>169.63869090061499</v>
+      </c>
+      <c r="F6">
+        <v>167.66403249363901</v>
+      </c>
+      <c r="G6">
         <v>177.05652595155999</v>
       </c>
-      <c r="F6">
-        <v>174.35339002358799</v>
-      </c>
-      <c r="G6">
-        <v>148.84774920772401</v>
-      </c>
       <c r="H6">
-        <v>168.781895563901</v>
+        <v>111.667058933801</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1089,16 +1074,16 @@
         <v>161.28250837355699</v>
       </c>
       <c r="E7">
+        <v>163.33974016018399</v>
+      </c>
+      <c r="F7">
+        <v>137.352321014621</v>
+      </c>
+      <c r="G7">
         <v>176.64454092941699</v>
       </c>
-      <c r="F7">
-        <v>150.26062109313901</v>
-      </c>
-      <c r="G7">
-        <v>164.214256204099</v>
-      </c>
       <c r="H7">
-        <v>163.33974016018399</v>
+        <v>99.336366849491199</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1115,16 +1100,16 @@
         <v>175.77970058956001</v>
       </c>
       <c r="E8">
+        <v>188.37665731786899</v>
+      </c>
+      <c r="F8">
+        <v>188.18478651228301</v>
+      </c>
+      <c r="G8">
         <v>196.14671968182401</v>
       </c>
-      <c r="F8">
-        <v>200.96664523627101</v>
-      </c>
-      <c r="G8">
-        <v>145.290597392763</v>
-      </c>
       <c r="H8">
-        <v>190.23238180563601</v>
+        <v>153.36845506933801</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1141,16 +1126,16 @@
         <v>170.740623275258</v>
       </c>
       <c r="E9">
+        <v>176.90253359114399</v>
+      </c>
+      <c r="F9">
+        <v>185.215418897229</v>
+      </c>
+      <c r="G9">
         <v>163.403429790389</v>
       </c>
-      <c r="F9">
-        <v>199.47420627699199</v>
-      </c>
-      <c r="G9">
-        <v>106.12786518495101</v>
-      </c>
       <c r="H9">
-        <v>184.93673870654399</v>
+        <v>171.236056857195</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1167,16 +1152,16 @@
         <v>200.802891864983</v>
       </c>
       <c r="E10">
+        <v>218.16563329876101</v>
+      </c>
+      <c r="F10">
+        <v>207.71562201206601</v>
+      </c>
+      <c r="G10">
         <v>223.61237750097999</v>
       </c>
-      <c r="F10">
-        <v>230.122224116372</v>
-      </c>
-      <c r="G10">
-        <v>152.30212612656501</v>
-      </c>
       <c r="H10">
-        <v>224.37578047420601</v>
+        <v>222.208126773977</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1193,16 +1178,16 @@
         <v>194.06375305394599</v>
       </c>
       <c r="E11">
+        <v>184.49988797670301</v>
+      </c>
+      <c r="F11">
+        <v>185.49069563343701</v>
+      </c>
+      <c r="G11">
         <v>203.82478139268699</v>
       </c>
-      <c r="F11">
-        <v>192.788358027898</v>
-      </c>
-      <c r="G11">
-        <v>145.77535398513899</v>
-      </c>
       <c r="H11">
-        <v>184.15961632167301</v>
+        <v>194.21733120044499</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1219,16 +1204,16 @@
         <v>224.51449533089101</v>
       </c>
       <c r="E12">
+        <v>229.24396631398699</v>
+      </c>
+      <c r="F12">
+        <v>236.275871325221</v>
+      </c>
+      <c r="G12">
         <v>285.60066246089099</v>
       </c>
-      <c r="F12">
-        <v>247.81520330192299</v>
-      </c>
-      <c r="G12">
-        <v>178.51728483914701</v>
-      </c>
       <c r="H12">
-        <v>226.59742937042799</v>
+        <v>220.44124604037501</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1245,16 +1230,16 @@
         <v>194.69853187920501</v>
       </c>
       <c r="E13">
+        <v>200.00821128259301</v>
+      </c>
+      <c r="F13">
+        <v>193.00544829518901</v>
+      </c>
+      <c r="G13">
         <v>183.64198796750699</v>
       </c>
-      <c r="F13">
-        <v>216.41437791515099</v>
-      </c>
-      <c r="G13">
-        <v>110.355276946895</v>
-      </c>
       <c r="H13">
-        <v>213.08423249139599</v>
+        <v>183.19314521500601</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1271,16 +1256,16 @@
         <v>205.43368567682799</v>
       </c>
       <c r="E14">
+        <v>254.55108581009199</v>
+      </c>
+      <c r="F14">
+        <v>248.51399141977299</v>
+      </c>
+      <c r="G14">
         <v>258.95650854404801</v>
       </c>
-      <c r="F14">
-        <v>259.84407671655799</v>
-      </c>
-      <c r="G14">
-        <v>153.75781591509599</v>
-      </c>
       <c r="H14">
-        <v>244.015758736511</v>
+        <v>153.674880067343</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1297,16 +1282,16 @@
         <v>218.96110964616801</v>
       </c>
       <c r="E15">
+        <v>222.26461463709001</v>
+      </c>
+      <c r="F15">
+        <v>200.95041121527899</v>
+      </c>
+      <c r="G15">
         <v>259.38040224172897</v>
       </c>
-      <c r="F15">
-        <v>224.649498464391</v>
-      </c>
-      <c r="G15">
-        <v>167.296952154667</v>
-      </c>
       <c r="H15">
-        <v>229.21209625802501</v>
+        <v>206.77466896264701</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1323,16 +1308,16 @@
         <v>212.16060908858699</v>
       </c>
       <c r="E16">
+        <v>253.03723073549</v>
+      </c>
+      <c r="F16">
+        <v>266.55759534308697</v>
+      </c>
+      <c r="G16">
         <v>259.129505582668</v>
       </c>
-      <c r="F16">
-        <v>280.23634866334697</v>
-      </c>
-      <c r="G16">
-        <v>158.454285702947</v>
-      </c>
       <c r="H16">
-        <v>263.63408363480301</v>
+        <v>183.48609194329299</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1340,22 +1325,22 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1370,18 +1355,18 @@
       </c>
       <c r="D22" s="1">
         <f>MEDIAN(B2:H2)</f>
-        <v>257.23306705018803</v>
+        <v>207.42057784644101</v>
       </c>
       <c r="E22">
         <f>ABS(B22-D22)</f>
-        <v>109.23306705018803</v>
+        <v>59.420577846441006</v>
       </c>
       <c r="F22" t="b">
-        <f>ABS(D22-B22)&lt;ABS(C22-B22)</f>
+        <f t="shared" ref="F22:F35" si="0">ABS(D22-B22)&lt;ABS(C22-B22)</f>
         <v>0</v>
       </c>
       <c r="G22" s="2" t="b">
-        <f>(D22-C22)*(B22-C22)&gt;0</f>
+        <f t="shared" ref="G22:G35" si="1">(D22-C22)*(B22-C22)&gt;0</f>
         <v>0</v>
       </c>
     </row>
@@ -1396,19 +1381,19 @@
         <v>120</v>
       </c>
       <c r="D23" s="1">
-        <f>MEDIAN(B3:H3)</f>
-        <v>149.857344546608</v>
+        <f t="shared" ref="D23:D36" si="2">MEDIAN(B3:H3)</f>
+        <v>149.34295628759699</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:E35" si="0">ABS(B23-D23)</f>
-        <v>54.142655453391995</v>
+        <f t="shared" ref="E23:E35" si="3">ABS(B23-D23)</f>
+        <v>54.657043712403009</v>
       </c>
       <c r="F23" t="b">
-        <f>ABS(D23-B23)&lt;ABS(C23-B23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G23" s="2" t="b">
-        <f>(D23-C23)*(B23-C23)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1423,19 +1408,19 @@
         <v>185</v>
       </c>
       <c r="D24" s="1">
-        <f>MEDIAN(B4:H4)</f>
-        <v>199.60767102854501</v>
+        <f t="shared" si="2"/>
+        <v>193.68009710486101</v>
       </c>
       <c r="E24">
+        <f t="shared" si="3"/>
+        <v>9.3199028951389948</v>
+      </c>
+      <c r="F24" t="b">
         <f t="shared" si="0"/>
-        <v>3.3923289714549867</v>
-      </c>
-      <c r="F24" t="b">
-        <f>ABS(D24-B24)&lt;ABS(C24-B24)</f>
         <v>1</v>
       </c>
       <c r="G24" s="2" t="b">
-        <f>(D24-C24)*(B24-C24)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1450,19 +1435,19 @@
         <v>197</v>
       </c>
       <c r="D25" s="1">
-        <f>MEDIAN(B5:H5)</f>
+        <f t="shared" si="2"/>
         <v>156.913746826991</v>
       </c>
       <c r="E25">
+        <f t="shared" si="3"/>
+        <v>82.913746826991002</v>
+      </c>
+      <c r="F25" t="b">
         <f t="shared" si="0"/>
-        <v>82.913746826991002</v>
-      </c>
-      <c r="F25" t="b">
-        <f>ABS(D25-B25)&lt;ABS(C25-B25)</f>
         <v>1</v>
       </c>
       <c r="G25" s="2" t="b">
-        <f>(D25-C25)*(B25-C25)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1477,19 +1462,19 @@
         <v>180</v>
       </c>
       <c r="D26" s="1">
-        <f>MEDIAN(B6:H6)</f>
-        <v>168.781895563901</v>
+        <f t="shared" si="2"/>
+        <v>168.67712586726799</v>
       </c>
       <c r="E26">
+        <f t="shared" si="3"/>
+        <v>55.677125867267989</v>
+      </c>
+      <c r="F26" t="b">
         <f t="shared" si="0"/>
-        <v>55.781895563901003</v>
-      </c>
-      <c r="F26" t="b">
-        <f>ABS(D26-B26)&lt;ABS(C26-B26)</f>
         <v>1</v>
       </c>
       <c r="G26" s="2" t="b">
-        <f>(D26-C26)*(B26-C26)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1504,19 +1489,19 @@
         <v>148.5</v>
       </c>
       <c r="D27" s="1">
-        <f>MEDIAN(B7:H7)</f>
-        <v>164.17774808403601</v>
+        <f t="shared" si="2"/>
+        <v>163.33974016018399</v>
       </c>
       <c r="E27">
+        <f t="shared" si="3"/>
+        <v>11.660259839816007</v>
+      </c>
+      <c r="F27" t="b">
         <f t="shared" si="0"/>
-        <v>10.822251915963989</v>
-      </c>
-      <c r="F27" t="b">
-        <f>ABS(D27-B27)&lt;ABS(C27-B27)</f>
         <v>1</v>
       </c>
       <c r="G27" s="2" t="b">
-        <f>(D27-C27)*(B27-C27)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1531,19 +1516,19 @@
         <v>200</v>
       </c>
       <c r="D28" s="1">
-        <f>MEDIAN(B8:H8)</f>
+        <f t="shared" si="2"/>
         <v>180.376594388538</v>
       </c>
       <c r="E28">
+        <f t="shared" si="3"/>
+        <v>11.623405611462005</v>
+      </c>
+      <c r="F28" t="b">
         <f t="shared" si="0"/>
-        <v>11.623405611462005</v>
-      </c>
-      <c r="F28" t="b">
-        <f>ABS(D28-B28)&lt;ABS(C28-B28)</f>
         <v>0</v>
       </c>
       <c r="G28" s="2" t="b">
-        <f>(D28-C28)*(B28-C28)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1558,19 +1543,19 @@
         <v>217.5</v>
       </c>
       <c r="D29" s="1">
-        <f>MEDIAN(B9:H9)</f>
-        <v>179.90517372004601</v>
+        <f t="shared" si="2"/>
+        <v>176.90253359114399</v>
       </c>
       <c r="E29">
+        <f t="shared" si="3"/>
+        <v>111.09746640885601</v>
+      </c>
+      <c r="F29" t="b">
         <f t="shared" si="0"/>
-        <v>108.09482627995399</v>
-      </c>
-      <c r="F29" t="b">
-        <f>ABS(D29-B29)&lt;ABS(C29-B29)</f>
         <v>0</v>
       </c>
       <c r="G29" s="2" t="b">
-        <f>(D29-C29)*(B29-C29)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1585,19 +1570,19 @@
         <v>215</v>
       </c>
       <c r="D30" s="1">
-        <f>MEDIAN(B10:H10)</f>
-        <v>201.48769078476101</v>
+        <f t="shared" si="2"/>
+        <v>207.71562201206601</v>
       </c>
       <c r="E30">
+        <f t="shared" si="3"/>
+        <v>9.2843779879339934</v>
+      </c>
+      <c r="F30" t="b">
         <f t="shared" si="0"/>
-        <v>15.512309215238986</v>
-      </c>
-      <c r="F30" t="b">
-        <f>ABS(D30-B30)&lt;ABS(C30-B30)</f>
         <v>0</v>
       </c>
       <c r="G30" s="2" t="b">
-        <f>(D30-C30)*(B30-C30)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1612,19 +1597,19 @@
         <v>215</v>
       </c>
       <c r="D31" s="1">
-        <f>MEDIAN(B11:H11)</f>
-        <v>194.06375305394599</v>
+        <f t="shared" si="2"/>
+        <v>194.21733120044499</v>
       </c>
       <c r="E31">
+        <f t="shared" si="3"/>
+        <v>93.782668799555012</v>
+      </c>
+      <c r="F31" t="b">
         <f t="shared" si="0"/>
-        <v>93.936246946054013</v>
-      </c>
-      <c r="F31" t="b">
-        <f>ABS(D31-B31)&lt;ABS(C31-B31)</f>
         <v>0</v>
       </c>
       <c r="G31" s="2" t="b">
-        <f>(D31-C31)*(B31-C31)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1639,19 +1624,19 @@
         <v>235</v>
       </c>
       <c r="D32" s="1">
-        <f>MEDIAN(B12:H12)</f>
+        <f t="shared" si="2"/>
         <v>224.51449533089101</v>
       </c>
       <c r="E32">
+        <f t="shared" si="3"/>
+        <v>15.514495330891009</v>
+      </c>
+      <c r="F32" t="b">
         <f t="shared" si="0"/>
-        <v>15.514495330891009</v>
-      </c>
-      <c r="F32" t="b">
-        <f>ABS(D32-B32)&lt;ABS(C32-B32)</f>
         <v>1</v>
       </c>
       <c r="G32" s="2" t="b">
-        <f>(D32-C32)*(B32-C32)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1666,19 +1651,19 @@
         <v>226</v>
       </c>
       <c r="D33" s="1">
-        <f>MEDIAN(B13:H13)</f>
-        <v>213.08423249139599</v>
+        <f t="shared" si="2"/>
+        <v>194.69853187920501</v>
       </c>
       <c r="E33">
+        <f t="shared" si="3"/>
+        <v>52.698531879205007</v>
+      </c>
+      <c r="F33" t="b">
         <f t="shared" si="0"/>
-        <v>71.084232491395994</v>
-      </c>
-      <c r="F33" t="b">
-        <f>ABS(D33-B33)&lt;ABS(C33-B33)</f>
         <v>1</v>
       </c>
       <c r="G33" s="2" t="b">
-        <f>(D33-C33)*(B33-C33)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1693,19 +1678,19 @@
         <v>215</v>
       </c>
       <c r="D34" s="1">
-        <f>MEDIAN(B14:H14)</f>
+        <f t="shared" si="2"/>
         <v>215.08812113530101</v>
       </c>
       <c r="E34">
+        <f t="shared" si="3"/>
+        <v>32.911878864698991</v>
+      </c>
+      <c r="F34" t="b">
         <f t="shared" si="0"/>
-        <v>32.911878864698991</v>
-      </c>
-      <c r="F34" t="b">
-        <f>ABS(D34-B34)&lt;ABS(C34-B34)</f>
         <v>1</v>
       </c>
       <c r="G34" s="2" t="b">
-        <f>(D34-C34)*(B34-C34)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1720,19 +1705,19 @@
         <v>231</v>
       </c>
       <c r="D35" s="1">
-        <f>MEDIAN(B15:H15)</f>
-        <v>229.21209625802501</v>
+        <f t="shared" si="2"/>
+        <v>222.26461463709001</v>
       </c>
       <c r="E35">
+        <f t="shared" si="3"/>
+        <v>8.2646146370900055</v>
+      </c>
+      <c r="F35" t="b">
         <f t="shared" si="0"/>
-        <v>15.212096258025014</v>
-      </c>
-      <c r="F35" t="b">
-        <f>ABS(D35-B35)&lt;ABS(C35-B35)</f>
         <v>1</v>
       </c>
       <c r="G35" s="2" t="b">
-        <f>(D35-C35)*(B35-C35)&gt;0</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1741,53 +1726,419 @@
         <v>201411</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C36">
         <v>230</v>
       </c>
-      <c r="D36" s="3">
-        <f>MEDIAN(B16:H16)</f>
+      <c r="D36" s="1">
+        <f t="shared" si="2"/>
         <v>220.39303050015599</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>201309</v>
+      </c>
+      <c r="B39">
+        <v>148</v>
+      </c>
+      <c r="C39">
+        <v>180</v>
+      </c>
+      <c r="D39">
+        <v>114.617801119193</v>
+      </c>
+      <c r="E39">
+        <f>ABS(B39-D39)</f>
+        <v>33.382198880806996</v>
+      </c>
+      <c r="F39" t="b">
+        <f t="shared" ref="F39:F52" si="4">ABS(D39-B39)&lt;ABS(C39-B39)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="2" t="b">
+        <f t="shared" ref="G39:G52" si="5">(D39-C39)*(B39-C39)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>201310</v>
+      </c>
+      <c r="B40">
+        <v>204</v>
+      </c>
+      <c r="C40">
+        <v>120</v>
+      </c>
+      <c r="D40">
+        <v>121.092961742477</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ref="E40:E52" si="6">ABS(B40-D40)</f>
+        <v>82.907038257522998</v>
+      </c>
+      <c r="F40" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G40" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>201311</v>
+      </c>
+      <c r="B41">
+        <v>203</v>
+      </c>
+      <c r="C41">
+        <v>185</v>
+      </c>
+      <c r="D41">
+        <v>130.93213212104001</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="6"/>
+        <v>72.067867878959987</v>
+      </c>
+      <c r="F41" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G41" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>201312</v>
+      </c>
+      <c r="B42">
+        <v>74</v>
+      </c>
+      <c r="C42">
+        <v>197</v>
+      </c>
+      <c r="D42">
+        <v>205.22140063756899</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="6"/>
+        <v>131.22140063756899</v>
+      </c>
+      <c r="F42" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G42" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>201401</v>
+      </c>
+      <c r="B43">
+        <v>113</v>
+      </c>
+      <c r="C43">
+        <v>180</v>
+      </c>
+      <c r="D43">
+        <v>213.09873569996199</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="6"/>
+        <v>100.09873569996199</v>
+      </c>
+      <c r="F43" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G43" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>201402</v>
+      </c>
+      <c r="B44">
+        <v>175</v>
+      </c>
+      <c r="C44">
+        <v>148.5</v>
+      </c>
+      <c r="D44">
+        <v>158.315327489769</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="6"/>
+        <v>16.684672510230996</v>
+      </c>
+      <c r="F44" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G44" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>201403</v>
+      </c>
+      <c r="B45">
+        <v>192</v>
+      </c>
+      <c r="C45">
+        <v>200</v>
+      </c>
+      <c r="D45">
+        <v>138.57674908568401</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="6"/>
+        <v>53.423250914315986</v>
+      </c>
+      <c r="F45" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G45" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>201404</v>
+      </c>
+      <c r="B46">
+        <v>288</v>
+      </c>
+      <c r="C46">
+        <v>217.5</v>
+      </c>
+      <c r="D46">
+        <v>210.09825613304301</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="6"/>
+        <v>77.901743866956991</v>
+      </c>
+      <c r="F46" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G46" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>201405</v>
+      </c>
+      <c r="B47">
+        <v>217</v>
+      </c>
+      <c r="C47">
+        <v>215</v>
+      </c>
+      <c r="D47">
+        <v>185.61843007688501</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="6"/>
+        <v>31.381569923114995</v>
+      </c>
+      <c r="F47" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>201406</v>
+      </c>
+      <c r="B48">
+        <v>288</v>
+      </c>
+      <c r="C48">
+        <v>215</v>
+      </c>
+      <c r="D48">
+        <v>218.80441090261601</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="6"/>
+        <v>69.195589097383987</v>
+      </c>
+      <c r="F48" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>201407</v>
+      </c>
+      <c r="B49">
+        <v>209</v>
+      </c>
+      <c r="C49">
+        <v>235</v>
+      </c>
+      <c r="D49">
+        <v>286.28765341114098</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="6"/>
+        <v>77.28765341114098</v>
+      </c>
+      <c r="F49" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>201408</v>
+      </c>
+      <c r="B50">
+        <v>142</v>
+      </c>
+      <c r="C50">
+        <v>226</v>
+      </c>
+      <c r="D50">
+        <v>295.38436350159498</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="6"/>
+        <v>153.38436350159498</v>
+      </c>
+      <c r="F50" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G50" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>201409</v>
+      </c>
+      <c r="B51">
+        <v>248</v>
+      </c>
+      <c r="C51">
+        <v>215</v>
+      </c>
+      <c r="D51">
+        <v>242.17785806620299</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="6"/>
+        <v>5.8221419337970133</v>
+      </c>
+      <c r="F51" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G51" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>201410</v>
+      </c>
+      <c r="B52">
+        <v>214</v>
+      </c>
+      <c r="C52">
+        <v>231</v>
+      </c>
+      <c r="D52">
+        <v>238.87001520548</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="6"/>
+        <v>24.870015205480001</v>
+      </c>
+      <c r="F52" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>201411</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>230</v>
+      </c>
+      <c r="D53">
+        <v>238.69452808186</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>